<commit_message>
Enhance logging and error handling for XTTS v2 model initialization in TTSWorker
</commit_message>
<xml_diff>
--- a/Classeur1.xlsx
+++ b/Classeur1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JF30LB\Projects\python\Projects\text_to_audio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4995180A-5235-4D00-ADD6-B1EAEC729D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB90047-E533-4487-9A14-787CEEDF027F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25305" yWindow="390" windowWidth="12810" windowHeight="15135" xr2:uid="{1ADD047B-3AB9-450D-966F-48F37E3C9FE2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
   <si>
     <t>Anglais</t>
   </si>
@@ -92,9 +92,6 @@
     <t>OK</t>
   </si>
   <si>
-    <t>femme</t>
-  </si>
-  <si>
     <t>pas terrible</t>
   </si>
   <si>
@@ -117,6 +114,15 @@
   </si>
   <si>
     <t>Erreur : Model is multi-speaker but no `speaker` is provided.</t>
+  </si>
+  <si>
+    <t>Homme</t>
+  </si>
+  <si>
+    <t>Femme</t>
+  </si>
+  <si>
+    <t>Own voice (français)</t>
   </si>
 </sst>
 </file>
@@ -491,7 +497,7 @@
   <dimension ref="B4:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,6 +505,7 @@
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
@@ -512,7 +519,7 @@
         <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
@@ -523,7 +530,7 @@
         <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
@@ -534,10 +541,10 @@
         <v>17</v>
       </c>
       <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" t="s">
         <v>18</v>
-      </c>
-      <c r="G6" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
@@ -545,13 +552,13 @@
         <v>4</v>
       </c>
       <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" t="s">
         <v>20</v>
-      </c>
-      <c r="F7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
@@ -559,13 +566,13 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -576,13 +583,13 @@
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" t="s">
         <v>23</v>
-      </c>
-      <c r="G9" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -590,13 +597,13 @@
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
@@ -607,10 +614,10 @@
         <v>17</v>
       </c>
       <c r="F11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" t="s">
         <v>18</v>
-      </c>
-      <c r="G11" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -618,13 +625,13 @@
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
@@ -638,13 +645,13 @@
         <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
@@ -652,13 +659,13 @@
         <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F14" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
@@ -666,13 +673,13 @@
         <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F15" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
@@ -680,13 +687,13 @@
         <v>15</v>
       </c>
       <c r="E16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F16" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.25">
@@ -694,13 +701,13 @@
         <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F17" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>